<commit_message>
added nbt mbp datasheet
</commit_message>
<xml_diff>
--- a/DataSheets/combined_nbt_mbpnls_24.xlsx
+++ b/DataSheets/combined_nbt_mbpnls_24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miramota/Desktop/Graphs/DataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940E8F56-CC1C-4D47-8578-69F6FFBE8034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45FF1AC-1A61-264C-92A2-F68441235FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{65CBED47-E614-884A-90FD-222407B7B541}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{65CBED47-E614-884A-90FD-222407B7B541}"/>
   </bookViews>
   <sheets>
     <sheet name="combined" sheetId="12" r:id="rId1"/>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F138" sqref="F138"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
edited condition values from strings to numerical
</commit_message>
<xml_diff>
--- a/DataSheets/combined_nbt_mbpnls_24.xlsx
+++ b/DataSheets/combined_nbt_mbpnls_24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miramota/Desktop/Graphs/DataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45FF1AC-1A61-264C-92A2-F68441235FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9BBFF9-7102-3F46-A736-CEA97842681C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{65CBED47-E614-884A-90FD-222407B7B541}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="274">
   <si>
     <t>neurons</t>
   </si>
@@ -845,9 +845,6 @@
     <t>condition</t>
   </si>
   <si>
-    <t>DMSO</t>
-  </si>
-  <si>
     <t>DMSO-WIN1-3_nbtdsred_mbp-nlscaax_5dpf_092824-01_AcquisitionBlock1_pt1-AP</t>
   </si>
   <si>
@@ -858,12 +855,6 @@
   </si>
   <si>
     <t>DMSO-WIN4_nbtdsred_mbp-nlscaax_5dpf_092824-01-AP</t>
-  </si>
-  <si>
-    <t>WIN05μM</t>
-  </si>
-  <si>
-    <t>WIN1μM</t>
   </si>
   <si>
     <t>rep maybe</t>
@@ -1346,7 +1337,7 @@
   <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1381,8 +1372,8 @@
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>268</v>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1398,8 +1389,8 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>268</v>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1415,8 +1406,8 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>268</v>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1432,8 +1423,8 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>268</v>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1449,8 +1440,8 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
-        <v>268</v>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1466,8 +1457,8 @@
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
-        <v>268</v>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1483,8 +1474,8 @@
       <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
-        <v>273</v>
+      <c r="E8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1500,8 +1491,8 @@
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
-        <v>273</v>
+      <c r="E9">
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1517,8 +1508,8 @@
       <c r="D10">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
-        <v>273</v>
+      <c r="E10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1534,8 +1525,8 @@
       <c r="D11">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>273</v>
+      <c r="E11">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1551,8 +1542,8 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>273</v>
+      <c r="E12">
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1568,8 +1559,8 @@
       <c r="D13">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
-        <v>273</v>
+      <c r="E13">
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1585,8 +1576,8 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>273</v>
+      <c r="E14">
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1602,8 +1593,8 @@
       <c r="D15">
         <v>3</v>
       </c>
-      <c r="E15" t="s">
-        <v>273</v>
+      <c r="E15">
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1619,8 +1610,8 @@
       <c r="D16">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
-        <v>274</v>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1636,8 +1627,8 @@
       <c r="D17">
         <v>3</v>
       </c>
-      <c r="E17" t="s">
-        <v>274</v>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1653,8 +1644,8 @@
       <c r="D18">
         <v>3</v>
       </c>
-      <c r="E18" t="s">
-        <v>274</v>
+      <c r="E18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1670,8 +1661,8 @@
       <c r="D19">
         <v>3</v>
       </c>
-      <c r="E19" t="s">
-        <v>274</v>
+      <c r="E19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1687,8 +1678,8 @@
       <c r="D20">
         <v>3</v>
       </c>
-      <c r="E20" t="s">
-        <v>274</v>
+      <c r="E20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1704,8 +1695,8 @@
       <c r="D21">
         <v>3</v>
       </c>
-      <c r="E21" t="s">
-        <v>274</v>
+      <c r="E21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1721,8 +1712,8 @@
       <c r="D22">
         <v>3</v>
       </c>
-      <c r="E22" t="s">
-        <v>274</v>
+      <c r="E22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1738,8 +1729,8 @@
       <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" t="s">
-        <v>274</v>
+      <c r="E23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1755,8 +1746,8 @@
       <c r="D24">
         <v>4</v>
       </c>
-      <c r="E24" t="s">
-        <v>268</v>
+      <c r="E24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1772,8 +1763,8 @@
       <c r="D25">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
-        <v>268</v>
+      <c r="E25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1789,8 +1780,8 @@
       <c r="D26">
         <v>4</v>
       </c>
-      <c r="E26" t="s">
-        <v>268</v>
+      <c r="E26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1806,8 +1797,8 @@
       <c r="D27">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
-        <v>268</v>
+      <c r="E27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1823,8 +1814,8 @@
       <c r="D28">
         <v>4</v>
       </c>
-      <c r="E28" t="s">
-        <v>268</v>
+      <c r="E28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1840,8 +1831,8 @@
       <c r="D29">
         <v>4</v>
       </c>
-      <c r="E29" t="s">
-        <v>268</v>
+      <c r="E29">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1857,8 +1848,8 @@
       <c r="D30">
         <v>4</v>
       </c>
-      <c r="E30" t="s">
-        <v>268</v>
+      <c r="E30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1874,8 +1865,8 @@
       <c r="D31">
         <v>4</v>
       </c>
-      <c r="E31" t="s">
-        <v>268</v>
+      <c r="E31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1891,8 +1882,8 @@
       <c r="D32">
         <v>4</v>
       </c>
-      <c r="E32" t="s">
-        <v>268</v>
+      <c r="E32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1908,8 +1899,8 @@
       <c r="D33">
         <v>4</v>
       </c>
-      <c r="E33" t="s">
-        <v>273</v>
+      <c r="E33">
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1925,8 +1916,8 @@
       <c r="D34" s="9">
         <v>4</v>
       </c>
-      <c r="E34" t="s">
-        <v>273</v>
+      <c r="E34">
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1942,8 +1933,8 @@
       <c r="D35">
         <v>4</v>
       </c>
-      <c r="E35" t="s">
-        <v>273</v>
+      <c r="E35">
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1959,8 +1950,8 @@
       <c r="D36">
         <v>4</v>
       </c>
-      <c r="E36" t="s">
-        <v>273</v>
+      <c r="E36">
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1976,8 +1967,8 @@
       <c r="D37">
         <v>4</v>
       </c>
-      <c r="E37" t="s">
-        <v>273</v>
+      <c r="E37">
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1993,8 +1984,8 @@
       <c r="D38">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
-        <v>273</v>
+      <c r="E38">
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2010,8 +2001,8 @@
       <c r="D39">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
-        <v>273</v>
+      <c r="E39">
+        <v>0.5</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2027,8 +2018,8 @@
       <c r="D40">
         <v>4</v>
       </c>
-      <c r="E40" t="s">
-        <v>273</v>
+      <c r="E40">
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2044,8 +2035,8 @@
       <c r="D41">
         <v>4</v>
       </c>
-      <c r="E41" t="s">
-        <v>274</v>
+      <c r="E41">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2061,8 +2052,8 @@
       <c r="D42">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
-        <v>274</v>
+      <c r="E42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2078,8 +2069,8 @@
       <c r="D43">
         <v>4</v>
       </c>
-      <c r="E43" t="s">
-        <v>274</v>
+      <c r="E43">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2095,8 +2086,8 @@
       <c r="D44">
         <v>4</v>
       </c>
-      <c r="E44" t="s">
-        <v>274</v>
+      <c r="E44">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2112,8 +2103,8 @@
       <c r="D45">
         <v>4</v>
       </c>
-      <c r="E45" t="s">
-        <v>274</v>
+      <c r="E45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2129,8 +2120,8 @@
       <c r="D46">
         <v>4</v>
       </c>
-      <c r="E46" t="s">
-        <v>274</v>
+      <c r="E46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2146,8 +2137,8 @@
       <c r="D47">
         <v>4</v>
       </c>
-      <c r="E47" t="s">
-        <v>274</v>
+      <c r="E47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2163,8 +2154,8 @@
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="E48" t="s">
-        <v>268</v>
+      <c r="E48">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2180,8 +2171,8 @@
       <c r="D49">
         <v>5</v>
       </c>
-      <c r="E49" t="s">
-        <v>268</v>
+      <c r="E49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2197,8 +2188,8 @@
       <c r="D50">
         <v>5</v>
       </c>
-      <c r="E50" t="s">
-        <v>268</v>
+      <c r="E50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2214,8 +2205,8 @@
       <c r="D51">
         <v>5</v>
       </c>
-      <c r="E51" t="s">
-        <v>268</v>
+      <c r="E51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2231,11 +2222,11 @@
       <c r="D52">
         <v>5</v>
       </c>
-      <c r="E52" t="s">
-        <v>268</v>
+      <c r="E52">
+        <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2251,8 +2242,8 @@
       <c r="D53">
         <v>5</v>
       </c>
-      <c r="E53" t="s">
-        <v>268</v>
+      <c r="E53">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2268,8 +2259,8 @@
       <c r="D54">
         <v>5</v>
       </c>
-      <c r="E54" t="s">
-        <v>268</v>
+      <c r="E54">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2285,8 +2276,8 @@
       <c r="D55">
         <v>5</v>
       </c>
-      <c r="E55" t="s">
-        <v>273</v>
+      <c r="E55">
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2302,8 +2293,8 @@
       <c r="D56">
         <v>5</v>
       </c>
-      <c r="E56" t="s">
-        <v>273</v>
+      <c r="E56">
+        <v>0.5</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2319,8 +2310,8 @@
       <c r="D57">
         <v>5</v>
       </c>
-      <c r="E57" t="s">
-        <v>273</v>
+      <c r="E57">
+        <v>0.5</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2336,8 +2327,8 @@
       <c r="D58">
         <v>5</v>
       </c>
-      <c r="E58" t="s">
-        <v>273</v>
+      <c r="E58">
+        <v>0.5</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -2353,8 +2344,8 @@
       <c r="D59">
         <v>5</v>
       </c>
-      <c r="E59" t="s">
-        <v>273</v>
+      <c r="E59">
+        <v>0.5</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2370,8 +2361,8 @@
       <c r="D60">
         <v>5</v>
       </c>
-      <c r="E60" t="s">
-        <v>273</v>
+      <c r="E60">
+        <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2387,8 +2378,8 @@
       <c r="D61">
         <v>5</v>
       </c>
-      <c r="E61" t="s">
-        <v>273</v>
+      <c r="E61">
+        <v>0.5</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2404,8 +2395,8 @@
       <c r="D62">
         <v>5</v>
       </c>
-      <c r="E62" t="s">
-        <v>273</v>
+      <c r="E62">
+        <v>0.5</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2421,8 +2412,8 @@
       <c r="D63">
         <v>5</v>
       </c>
-      <c r="E63" t="s">
-        <v>273</v>
+      <c r="E63">
+        <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2438,8 +2429,8 @@
       <c r="D64">
         <v>5</v>
       </c>
-      <c r="E64" t="s">
-        <v>274</v>
+      <c r="E64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2455,8 +2446,8 @@
       <c r="D65">
         <v>5</v>
       </c>
-      <c r="E65" t="s">
-        <v>274</v>
+      <c r="E65">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2472,8 +2463,8 @@
       <c r="D66">
         <v>5</v>
       </c>
-      <c r="E66" t="s">
-        <v>274</v>
+      <c r="E66">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2489,8 +2480,8 @@
       <c r="D67">
         <v>5</v>
       </c>
-      <c r="E67" t="s">
-        <v>274</v>
+      <c r="E67">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2506,11 +2497,11 @@
       <c r="D68">
         <v>5</v>
       </c>
-      <c r="E68" t="s">
-        <v>274</v>
+      <c r="E68">
+        <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2526,8 +2517,8 @@
       <c r="D69">
         <v>5</v>
       </c>
-      <c r="E69" t="s">
-        <v>274</v>
+      <c r="E69">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2543,8 +2534,8 @@
       <c r="D70">
         <v>5</v>
       </c>
-      <c r="E70" t="s">
-        <v>274</v>
+      <c r="E70">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2560,8 +2551,8 @@
       <c r="D71" s="1">
         <v>3</v>
       </c>
-      <c r="E71" t="s">
-        <v>268</v>
+      <c r="E71">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2577,8 +2568,8 @@
       <c r="D72" s="1">
         <v>3</v>
       </c>
-      <c r="E72" t="s">
-        <v>273</v>
+      <c r="E72">
+        <v>0.5</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2594,8 +2585,8 @@
       <c r="D73" s="1">
         <v>3</v>
       </c>
-      <c r="E73" t="s">
-        <v>274</v>
+      <c r="E73">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2611,8 +2602,8 @@
       <c r="D74" s="1">
         <v>3</v>
       </c>
-      <c r="E74" t="s">
-        <v>274</v>
+      <c r="E74">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2628,8 +2619,8 @@
       <c r="D75" s="1">
         <v>3</v>
       </c>
-      <c r="E75" t="s">
-        <v>274</v>
+      <c r="E75">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2645,8 +2636,8 @@
       <c r="D76">
         <v>4</v>
       </c>
-      <c r="E76" t="s">
-        <v>268</v>
+      <c r="E76">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2662,8 +2653,8 @@
       <c r="D77">
         <v>4</v>
       </c>
-      <c r="E77" t="s">
-        <v>273</v>
+      <c r="E77">
+        <v>0.5</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2679,8 +2670,8 @@
       <c r="D78">
         <v>4</v>
       </c>
-      <c r="E78" t="s">
-        <v>274</v>
+      <c r="E78">
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -2696,8 +2687,8 @@
       <c r="D79">
         <v>4</v>
       </c>
-      <c r="E79" t="s">
-        <v>274</v>
+      <c r="E79">
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -2713,8 +2704,8 @@
       <c r="D80">
         <v>4</v>
       </c>
-      <c r="E80" t="s">
-        <v>274</v>
+      <c r="E80">
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2730,8 +2721,8 @@
       <c r="D81" s="11">
         <v>3</v>
       </c>
-      <c r="E81" t="s">
-        <v>268</v>
+      <c r="E81">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2747,8 +2738,8 @@
       <c r="D82" s="11">
         <v>3</v>
       </c>
-      <c r="E82" t="s">
-        <v>268</v>
+      <c r="E82">
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2764,8 +2755,8 @@
       <c r="D83" s="11">
         <v>3</v>
       </c>
-      <c r="E83" t="s">
-        <v>268</v>
+      <c r="E83">
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2781,8 +2772,8 @@
       <c r="D84" s="11">
         <v>3</v>
       </c>
-      <c r="E84" t="s">
-        <v>268</v>
+      <c r="E84">
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2798,8 +2789,8 @@
       <c r="D85" s="3">
         <v>3</v>
       </c>
-      <c r="E85" t="s">
-        <v>268</v>
+      <c r="E85">
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2815,8 +2806,8 @@
       <c r="D86" s="3">
         <v>3</v>
       </c>
-      <c r="E86" t="s">
-        <v>268</v>
+      <c r="E86">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2832,8 +2823,8 @@
       <c r="D87" s="4">
         <v>3</v>
       </c>
-      <c r="E87" t="s">
-        <v>273</v>
+      <c r="E87">
+        <v>0.5</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2849,8 +2840,8 @@
       <c r="D88" s="4">
         <v>3</v>
       </c>
-      <c r="E88" t="s">
-        <v>273</v>
+      <c r="E88">
+        <v>0.5</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2866,8 +2857,8 @@
       <c r="D89" s="4">
         <v>3</v>
       </c>
-      <c r="E89" t="s">
-        <v>273</v>
+      <c r="E89">
+        <v>0.5</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2883,8 +2874,8 @@
       <c r="D90" s="4">
         <v>3</v>
       </c>
-      <c r="E90" t="s">
-        <v>273</v>
+      <c r="E90">
+        <v>0.5</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2900,8 +2891,8 @@
       <c r="D91" s="4">
         <v>3</v>
       </c>
-      <c r="E91" t="s">
-        <v>273</v>
+      <c r="E91">
+        <v>0.5</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2917,8 +2908,8 @@
       <c r="D92" s="4">
         <v>3</v>
       </c>
-      <c r="E92" t="s">
-        <v>273</v>
+      <c r="E92">
+        <v>0.5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2934,8 +2925,8 @@
       <c r="D93" s="2">
         <v>3</v>
       </c>
-      <c r="E93" t="s">
-        <v>274</v>
+      <c r="E93">
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2951,8 +2942,8 @@
       <c r="D94" s="2">
         <v>3</v>
       </c>
-      <c r="E94" t="s">
-        <v>274</v>
+      <c r="E94">
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2968,8 +2959,8 @@
       <c r="D95" s="2">
         <v>3</v>
       </c>
-      <c r="E95" t="s">
-        <v>274</v>
+      <c r="E95">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2985,8 +2976,8 @@
       <c r="D96" s="2">
         <v>3</v>
       </c>
-      <c r="E96" t="s">
-        <v>274</v>
+      <c r="E96">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -3002,8 +2993,8 @@
       <c r="D97" s="2">
         <v>3</v>
       </c>
-      <c r="E97" t="s">
-        <v>274</v>
+      <c r="E97">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -3019,8 +3010,8 @@
       <c r="D98" s="2">
         <v>3</v>
       </c>
-      <c r="E98" t="s">
-        <v>274</v>
+      <c r="E98">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3036,8 +3027,8 @@
       <c r="D99" s="2">
         <v>3</v>
       </c>
-      <c r="E99" t="s">
-        <v>274</v>
+      <c r="E99">
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -3053,8 +3044,8 @@
       <c r="D100" s="2">
         <v>3</v>
       </c>
-      <c r="E100" t="s">
-        <v>274</v>
+      <c r="E100">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3070,8 +3061,8 @@
       <c r="D101" s="3">
         <v>4</v>
       </c>
-      <c r="E101" t="s">
-        <v>268</v>
+      <c r="E101">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -3087,8 +3078,8 @@
       <c r="D102" s="3">
         <v>4</v>
       </c>
-      <c r="E102" t="s">
-        <v>268</v>
+      <c r="E102">
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -3104,8 +3095,8 @@
       <c r="D103" s="3">
         <v>4</v>
       </c>
-      <c r="E103" t="s">
-        <v>268</v>
+      <c r="E103">
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -3121,8 +3112,8 @@
       <c r="D104" s="3">
         <v>4</v>
       </c>
-      <c r="E104" t="s">
-        <v>268</v>
+      <c r="E104">
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -3138,8 +3129,8 @@
       <c r="D105" s="3">
         <v>4</v>
       </c>
-      <c r="E105" t="s">
-        <v>268</v>
+      <c r="E105">
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -3155,8 +3146,8 @@
       <c r="D106" s="3">
         <v>4</v>
       </c>
-      <c r="E106" t="s">
-        <v>268</v>
+      <c r="E106">
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -3172,8 +3163,8 @@
       <c r="D107" s="4">
         <v>4</v>
       </c>
-      <c r="E107" t="s">
-        <v>273</v>
+      <c r="E107">
+        <v>0.5</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3189,8 +3180,8 @@
       <c r="D108" s="4">
         <v>4</v>
       </c>
-      <c r="E108" t="s">
-        <v>273</v>
+      <c r="E108">
+        <v>0.5</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -3206,8 +3197,8 @@
       <c r="D109" s="4">
         <v>4</v>
       </c>
-      <c r="E109" t="s">
-        <v>273</v>
+      <c r="E109">
+        <v>0.5</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3223,8 +3214,8 @@
       <c r="D110" s="4">
         <v>4</v>
       </c>
-      <c r="E110" t="s">
-        <v>273</v>
+      <c r="E110">
+        <v>0.5</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -3240,8 +3231,8 @@
       <c r="D111" s="4">
         <v>4</v>
       </c>
-      <c r="E111" t="s">
-        <v>273</v>
+      <c r="E111">
+        <v>0.5</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -3257,8 +3248,8 @@
       <c r="D112" s="2">
         <v>4</v>
       </c>
-      <c r="E112" t="s">
-        <v>274</v>
+      <c r="E112">
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -3274,8 +3265,8 @@
       <c r="D113" s="2">
         <v>4</v>
       </c>
-      <c r="E113" t="s">
-        <v>274</v>
+      <c r="E113">
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -3291,8 +3282,8 @@
       <c r="D114" s="2">
         <v>4</v>
       </c>
-      <c r="E114" t="s">
-        <v>274</v>
+      <c r="E114">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -3308,8 +3299,8 @@
       <c r="D115" s="2">
         <v>4</v>
       </c>
-      <c r="E115" t="s">
-        <v>274</v>
+      <c r="E115">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -3325,8 +3316,8 @@
       <c r="D116" s="2">
         <v>4</v>
       </c>
-      <c r="E116" t="s">
-        <v>274</v>
+      <c r="E116">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -3342,8 +3333,8 @@
       <c r="D117" s="2">
         <v>4</v>
       </c>
-      <c r="E117" t="s">
-        <v>274</v>
+      <c r="E117">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -3359,8 +3350,8 @@
       <c r="D118" s="2">
         <v>4</v>
       </c>
-      <c r="E118" t="s">
-        <v>274</v>
+      <c r="E118">
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -3376,8 +3367,8 @@
       <c r="D119" s="2">
         <v>4</v>
       </c>
-      <c r="E119" t="s">
-        <v>274</v>
+      <c r="E119">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -3393,11 +3384,11 @@
       <c r="D120" s="11">
         <v>5</v>
       </c>
-      <c r="E120" t="s">
-        <v>268</v>
+      <c r="E120">
+        <v>0</v>
       </c>
       <c r="F120" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -3413,8 +3404,8 @@
       <c r="D121" s="11">
         <v>5</v>
       </c>
-      <c r="E121" t="s">
-        <v>268</v>
+      <c r="E121">
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -3430,8 +3421,8 @@
       <c r="D122" s="11">
         <v>5</v>
       </c>
-      <c r="E122" t="s">
-        <v>268</v>
+      <c r="E122">
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -3447,8 +3438,8 @@
       <c r="D123" s="11">
         <v>5</v>
       </c>
-      <c r="E123" t="s">
-        <v>268</v>
+      <c r="E123">
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -3464,11 +3455,11 @@
       <c r="D124" s="11">
         <v>5</v>
       </c>
-      <c r="E124" t="s">
-        <v>268</v>
+      <c r="E124">
+        <v>0</v>
       </c>
       <c r="F124" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -3484,8 +3475,8 @@
       <c r="D125" s="11">
         <v>5</v>
       </c>
-      <c r="E125" t="s">
-        <v>268</v>
+      <c r="E125">
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -3501,8 +3492,8 @@
       <c r="D126" s="13">
         <v>5</v>
       </c>
-      <c r="E126" t="s">
-        <v>273</v>
+      <c r="E126">
+        <v>0.5</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -3518,8 +3509,8 @@
       <c r="D127" s="13">
         <v>5</v>
       </c>
-      <c r="E127" t="s">
-        <v>273</v>
+      <c r="E127">
+        <v>0.5</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -3535,8 +3526,8 @@
       <c r="D128" s="13">
         <v>5</v>
       </c>
-      <c r="E128" t="s">
-        <v>273</v>
+      <c r="E128">
+        <v>0.5</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -3552,8 +3543,8 @@
       <c r="D129" s="13">
         <v>5</v>
       </c>
-      <c r="E129" t="s">
-        <v>273</v>
+      <c r="E129">
+        <v>0.5</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -3569,8 +3560,8 @@
       <c r="D130" s="13">
         <v>5</v>
       </c>
-      <c r="E130" t="s">
-        <v>273</v>
+      <c r="E130">
+        <v>0.5</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -3586,11 +3577,11 @@
       <c r="D131" s="14">
         <v>5</v>
       </c>
-      <c r="E131" t="s">
-        <v>274</v>
+      <c r="E131">
+        <v>1</v>
       </c>
       <c r="F131" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -3606,8 +3597,8 @@
       <c r="D132" s="14">
         <v>5</v>
       </c>
-      <c r="E132" t="s">
-        <v>274</v>
+      <c r="E132">
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -3623,8 +3614,8 @@
       <c r="D133" s="14">
         <v>5</v>
       </c>
-      <c r="E133" t="s">
-        <v>274</v>
+      <c r="E133">
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -3640,8 +3631,8 @@
       <c r="D134" s="14">
         <v>5</v>
       </c>
-      <c r="E134" t="s">
-        <v>274</v>
+      <c r="E134">
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -3657,8 +3648,8 @@
       <c r="D135" s="14">
         <v>5</v>
       </c>
-      <c r="E135" t="s">
-        <v>274</v>
+      <c r="E135">
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -3674,8 +3665,8 @@
       <c r="D136" s="14">
         <v>5</v>
       </c>
-      <c r="E136" t="s">
-        <v>274</v>
+      <c r="E136">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
@@ -3691,8 +3682,8 @@
       <c r="D137" s="14">
         <v>5</v>
       </c>
-      <c r="E137" t="s">
-        <v>274</v>
+      <c r="E137">
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -3708,11 +3699,11 @@
       <c r="D138" s="14">
         <v>5</v>
       </c>
-      <c r="E138" t="s">
-        <v>274</v>
+      <c r="E138">
+        <v>1</v>
       </c>
       <c r="F138" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
@@ -3728,8 +3719,8 @@
       <c r="D139">
         <v>5</v>
       </c>
-      <c r="E139" t="s">
-        <v>268</v>
+      <c r="E139">
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -3745,8 +3736,8 @@
       <c r="D140">
         <v>5</v>
       </c>
-      <c r="E140" t="s">
-        <v>273</v>
+      <c r="E140">
+        <v>0.5</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -3762,8 +3753,8 @@
       <c r="D141">
         <v>5</v>
       </c>
-      <c r="E141" t="s">
-        <v>274</v>
+      <c r="E141">
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -3779,8 +3770,8 @@
       <c r="D142">
         <v>5</v>
       </c>
-      <c r="E142" t="s">
-        <v>274</v>
+      <c r="E142">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5718,7 +5709,7 @@
         <v>4</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O2" s="8">
         <v>2</v>
@@ -5787,7 +5778,7 @@
         <v>4</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O4" s="4">
         <v>3</v>
@@ -5891,7 +5882,7 @@
         <v>4</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="O7" s="2">
         <v>9</v>
@@ -5944,7 +5935,7 @@
         <v>4</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O8" s="2">
         <v>7</v>
@@ -6339,7 +6330,7 @@
         <v>5</v>
       </c>
       <c r="S7" s="15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -7021,7 +7012,7 @@
         <v>5</v>
       </c>
       <c r="S23" s="15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">

</xml_diff>